<commit_message>
final edit - notebook, xlsx
</commit_message>
<xml_diff>
--- a/CPI_multiplier.xlsx
+++ b/CPI_multiplier.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bjane\flatiron-ds-course\module02\final_project\dsc-mod-2-project-v2-1-onl01-dtsc-ft-012120\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB683DFC-6411-4DE2-858D-C16E135A1576}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA88D425-83CA-4B2A-BBF6-61AAD970AD5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{3CA7DAAE-2C9C-41E8-889E-7743281F1D66}"/>
   </bookViews>
@@ -33,13 +33,28 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={430027AD-0D80-4FC6-BEC7-ED0804E637C8}</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{430027AD-0D80-4FC6-BEC7-ED0804E637C8}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    use to check price multiplier column - looks good</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Year</t>
-  </si>
-  <si>
-    <t>Annual Inflation</t>
   </si>
   <si>
     <t>Cost of Item</t>
@@ -50,6 +65,9 @@
   <si>
     <t>Price in 2019 Dollars</t>
   </si>
+  <si>
+    <t>Annual Inflation (%)</t>
+  </si>
 </sst>
 </file>
 
@@ -58,7 +76,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,6 +98,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -124,6 +148,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Braydon Janecek" id="{A43F7633-D423-421A-9FE7-54563E6A6A79}" userId="a477ba9231a48ded" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -421,12 +451,20 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="E1" dT="2020-03-25T17:24:40.60" personId="{A43F7633-D423-421A-9FE7-54563E6A6A79}" id="{430027AD-0D80-4FC6-BEC7-ED0804E637C8}">
+    <text>use to check price multiplier column - looks good</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA330AB3-1DA6-4A7D-B720-596937F4D089}">
   <dimension ref="B2:BM2"/>
   <sheetViews>
-    <sheetView topLeftCell="AQ1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:BM2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -632,16 +670,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D514A020-4FB3-49D0-A989-CCD805071B65}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D514A020-4FB3-49D0-A989-CCD805071B65}">
   <dimension ref="A1:E65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1"/>
@@ -652,16 +691,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1945,5 +1984,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>